<commit_message>
PCB complete and ordered
</commit_message>
<xml_diff>
--- a/Documents/eisendani_489-BOM order II.xlsx
+++ b/Documents/eisendani_489-BOM order II.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet_rec" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t xml:space="preserve">Supplier</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Qty. </t>
   </si>
   <si>
+    <t xml:space="preserve">Recieved</t>
+  </si>
+  <si>
     <t xml:space="preserve">Description</t>
   </si>
   <si>
@@ -106,19 +109,49 @@
     <t xml:space="preserve">Power Barrel Connector Jack 2.50mm ID (0.098"), 5.50mm OD (0.217") Through Hole, Right Angle</t>
   </si>
   <si>
-    <t xml:space="preserve">nano/small uC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Humidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Battery holder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">oled screen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pressure</t>
+    <t xml:space="preserve">1528-4884-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP2040 Feather series ARM® Cortex®-M0+ MCU 32-Bit Embedded Evaluation Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2648-SC0915CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC0915</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RP2040 Raspberry Pi Pico series ARM® Cortex®-M0+ MCU 32-Bit Embedded Evaluation Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pololu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRV8825</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stepper Motor Driver Carrier, Step/Dir, High Current, 1/32step, 1.5A/Phase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1528-1359-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BME280 series Humidity, Pressure, Temperature Sensor Evaluation Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1528-4650-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLED 1.3" Display Feather Platform Evaluation Expansion Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adafruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIPO 552530</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithium Ion Polymer Battery with Short Cable - 3.7V 350mAh</t>
   </si>
 </sst>
 </file>
@@ -155,20 +188,20 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -176,7 +209,7 @@
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -184,25 +217,35 @@
       <u val="single"/>
       <sz val="10"/>
       <color rgb="FF1155CC"/>
-      <name val="Arial"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <name val="arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00A933"/>
+        <bgColor rgb="FF008000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF993300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -221,7 +264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -245,10 +288,27 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -256,35 +316,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -299,43 +335,82 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Untitled1" xfId="20"/>
+    <cellStyle name="Gottem" xfId="21"/>
+    <cellStyle name="Lostem" xfId="22"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00A933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -387,7 +462,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -404,3174 +479,3296 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA999"/>
+  <dimension ref="A1:AB999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.95"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="84.76"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="6" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="15.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="3" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9" t="n">
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="11"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="9" t="n">
+      <c r="E4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="13"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="10" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13"/>
+      <c r="D5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="17" t="n">
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="11" t="n">
         <f aca="false">(2*D3)+(4*D5)</f>
-        <v>16</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="8" t="s">
         <v>24</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="9" t="n">
+      <c r="C8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>4884</v>
+      </c>
+      <c r="D9" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="18"/>
-      <c r="E9" s="19" t="s">
-        <v>28</v>
+      <c r="E9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="18"/>
-      <c r="E10" s="19" t="s">
-        <v>29</v>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="18"/>
-      <c r="E11" s="19" t="s">
-        <v>30</v>
+      <c r="A11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>2133</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="18"/>
-      <c r="E12" s="19" t="s">
-        <v>31</v>
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <v>2652</v>
+      </c>
+      <c r="D12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="18"/>
-      <c r="E13" s="19" t="s">
-        <v>32</v>
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="13" t="n">
+        <v>4650</v>
+      </c>
+      <c r="D13" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="18"/>
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="15" t="n">
+        <v>4237</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="18"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C16" s="8"/>
+      <c r="E16" s="17"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="18"/>
+      <c r="C17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="18"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C19" s="18"/>
+      <c r="C18" s="8"/>
+    </row>
+    <row r="19" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="18"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="18"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="18"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="18"/>
+      <c r="C23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="18"/>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="18"/>
+      <c r="C25" s="8"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="18"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C27" s="18"/>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="18"/>
+      <c r="C28" s="8"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="18"/>
+      <c r="C29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="18"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="18"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="18"/>
+      <c r="C32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="18"/>
+      <c r="C33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="18"/>
+      <c r="C34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="18"/>
+      <c r="C35" s="8"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="18"/>
+      <c r="C36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="18"/>
+      <c r="C37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="18"/>
+      <c r="C38" s="8"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="18"/>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="18"/>
+      <c r="C40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="18"/>
+      <c r="C41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="18"/>
+      <c r="C42" s="8"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="18"/>
+      <c r="C43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="18"/>
+      <c r="C44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="18"/>
+      <c r="C45" s="8"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="18"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="18"/>
+      <c r="C47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="18"/>
+      <c r="C48" s="8"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="18"/>
+      <c r="C49" s="8"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="18"/>
+      <c r="C50" s="8"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="18"/>
+      <c r="C51" s="8"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="18"/>
+      <c r="C52" s="8"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="18"/>
+      <c r="C53" s="8"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="18"/>
+      <c r="C54" s="8"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="18"/>
+      <c r="C55" s="8"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="18"/>
+      <c r="C56" s="8"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="18"/>
+      <c r="C57" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="18"/>
+      <c r="C58" s="8"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="18"/>
+      <c r="C59" s="8"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="18"/>
+      <c r="C60" s="8"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="18"/>
+      <c r="C61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C62" s="18"/>
+      <c r="C62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="18"/>
+      <c r="C63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C64" s="18"/>
+      <c r="C64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="18"/>
+      <c r="C65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="18"/>
+      <c r="C66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="18"/>
+      <c r="C67" s="8"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="18"/>
+      <c r="C68" s="8"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C69" s="18"/>
+      <c r="C69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="18"/>
+      <c r="C70" s="8"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="18"/>
+      <c r="C71" s="8"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="18"/>
+      <c r="C72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C73" s="18"/>
+      <c r="C73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="18"/>
+      <c r="C74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C75" s="18"/>
+      <c r="C75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="18"/>
+      <c r="C76" s="8"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="18"/>
+      <c r="C77" s="8"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="18"/>
+      <c r="C78" s="8"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="18"/>
+      <c r="C79" s="8"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="18"/>
+      <c r="C80" s="8"/>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C81" s="18"/>
+      <c r="C81" s="8"/>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="18"/>
+      <c r="C82" s="8"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="18"/>
+      <c r="C83" s="8"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="18"/>
+      <c r="C84" s="8"/>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="18"/>
+      <c r="C85" s="8"/>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="18"/>
+      <c r="C86" s="8"/>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="18"/>
+      <c r="C87" s="8"/>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="18"/>
+      <c r="C88" s="8"/>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="18"/>
+      <c r="C89" s="8"/>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="18"/>
+      <c r="C90" s="8"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="18"/>
+      <c r="C91" s="8"/>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="18"/>
+      <c r="C92" s="8"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="18"/>
+      <c r="C93" s="8"/>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="18"/>
+      <c r="C94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="18"/>
+      <c r="C95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C96" s="18"/>
+      <c r="C96" s="8"/>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="18"/>
+      <c r="C97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="18"/>
+      <c r="C98" s="8"/>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="18"/>
+      <c r="C99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C100" s="18"/>
+      <c r="C100" s="8"/>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="18"/>
+      <c r="C101" s="8"/>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="18"/>
+      <c r="C102" s="8"/>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="18"/>
+      <c r="C103" s="8"/>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="18"/>
+      <c r="C104" s="8"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="18"/>
+      <c r="C105" s="8"/>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C106" s="18"/>
+      <c r="C106" s="8"/>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="18"/>
+      <c r="C107" s="8"/>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="18"/>
+      <c r="C108" s="8"/>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C109" s="18"/>
+      <c r="C109" s="8"/>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="18"/>
+      <c r="C110" s="8"/>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="18"/>
+      <c r="C111" s="8"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="18"/>
+      <c r="C112" s="8"/>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C113" s="18"/>
+      <c r="C113" s="8"/>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="18"/>
+      <c r="C114" s="8"/>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="18"/>
+      <c r="C115" s="8"/>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="18"/>
+      <c r="C116" s="8"/>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="18"/>
+      <c r="C117" s="8"/>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="18"/>
+      <c r="C118" s="8"/>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="18"/>
+      <c r="C119" s="8"/>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="18"/>
+      <c r="C120" s="8"/>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="18"/>
+      <c r="C121" s="8"/>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="18"/>
+      <c r="C122" s="8"/>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C123" s="18"/>
+      <c r="C123" s="8"/>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C124" s="18"/>
+      <c r="C124" s="8"/>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C125" s="18"/>
+      <c r="C125" s="8"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="18"/>
+      <c r="C126" s="8"/>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="18"/>
+      <c r="C127" s="8"/>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="18"/>
+      <c r="C128" s="8"/>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C129" s="18"/>
+      <c r="C129" s="8"/>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C130" s="18"/>
+      <c r="C130" s="8"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="18"/>
+      <c r="C131" s="8"/>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="18"/>
+      <c r="C132" s="8"/>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C133" s="18"/>
+      <c r="C133" s="8"/>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="18"/>
+      <c r="C134" s="8"/>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="18"/>
+      <c r="C135" s="8"/>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C136" s="18"/>
+      <c r="C136" s="8"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C137" s="18"/>
+      <c r="C137" s="8"/>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C138" s="18"/>
+      <c r="C138" s="8"/>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="18"/>
+      <c r="C139" s="8"/>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C140" s="18"/>
+      <c r="C140" s="8"/>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C141" s="18"/>
+      <c r="C141" s="8"/>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C142" s="18"/>
+      <c r="C142" s="8"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="18"/>
+      <c r="C143" s="8"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C144" s="18"/>
+      <c r="C144" s="8"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C145" s="18"/>
+      <c r="C145" s="8"/>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C146" s="18"/>
+      <c r="C146" s="8"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="18"/>
+      <c r="C147" s="8"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="18"/>
+      <c r="C148" s="8"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C149" s="18"/>
+      <c r="C149" s="8"/>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C150" s="18"/>
+      <c r="C150" s="8"/>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="18"/>
+      <c r="C151" s="8"/>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="18"/>
+      <c r="C152" s="8"/>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="18"/>
+      <c r="C153" s="8"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="18"/>
+      <c r="C154" s="8"/>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="18"/>
+      <c r="C155" s="8"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C156" s="18"/>
+      <c r="C156" s="8"/>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="18"/>
+      <c r="C157" s="8"/>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C158" s="18"/>
+      <c r="C158" s="8"/>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C159" s="18"/>
+      <c r="C159" s="8"/>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="18"/>
+      <c r="C160" s="8"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="18"/>
+      <c r="C161" s="8"/>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="18"/>
+      <c r="C162" s="8"/>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="18"/>
+      <c r="C163" s="8"/>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="18"/>
+      <c r="C164" s="8"/>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C165" s="18"/>
+      <c r="C165" s="8"/>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C166" s="18"/>
+      <c r="C166" s="8"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C167" s="18"/>
+      <c r="C167" s="8"/>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="18"/>
+      <c r="C168" s="8"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C169" s="18"/>
+      <c r="C169" s="8"/>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="18"/>
+      <c r="C170" s="8"/>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="18"/>
+      <c r="C171" s="8"/>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="18"/>
+      <c r="C172" s="8"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="18"/>
+      <c r="C173" s="8"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C174" s="18"/>
+      <c r="C174" s="8"/>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="18"/>
+      <c r="C175" s="8"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C176" s="18"/>
+      <c r="C176" s="8"/>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C177" s="18"/>
+      <c r="C177" s="8"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="18"/>
+      <c r="C178" s="8"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C179" s="18"/>
+      <c r="C179" s="8"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C180" s="18"/>
+      <c r="C180" s="8"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="18"/>
+      <c r="C181" s="8"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="18"/>
+      <c r="C182" s="8"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="18"/>
+      <c r="C183" s="8"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C184" s="18"/>
+      <c r="C184" s="8"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="18"/>
+      <c r="C185" s="8"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="18"/>
+      <c r="C186" s="8"/>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C187" s="18"/>
+      <c r="C187" s="8"/>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C188" s="18"/>
+      <c r="C188" s="8"/>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C189" s="18"/>
+      <c r="C189" s="8"/>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C190" s="18"/>
+      <c r="C190" s="8"/>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C191" s="18"/>
+      <c r="C191" s="8"/>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C192" s="18"/>
+      <c r="C192" s="8"/>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C193" s="18"/>
+      <c r="C193" s="8"/>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="18"/>
+      <c r="C194" s="8"/>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="18"/>
+      <c r="C195" s="8"/>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C196" s="18"/>
+      <c r="C196" s="8"/>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C197" s="18"/>
+      <c r="C197" s="8"/>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C198" s="18"/>
+      <c r="C198" s="8"/>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="18"/>
+      <c r="C199" s="8"/>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="18"/>
+      <c r="C200" s="8"/>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C201" s="18"/>
+      <c r="C201" s="8"/>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C202" s="18"/>
+      <c r="C202" s="8"/>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="18"/>
+      <c r="C203" s="8"/>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="18"/>
+      <c r="C204" s="8"/>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C205" s="18"/>
+      <c r="C205" s="8"/>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="18"/>
+      <c r="C206" s="8"/>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="18"/>
+      <c r="C207" s="8"/>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C208" s="18"/>
+      <c r="C208" s="8"/>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C209" s="18"/>
+      <c r="C209" s="8"/>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="18"/>
+      <c r="C210" s="8"/>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C211" s="18"/>
+      <c r="C211" s="8"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C212" s="18"/>
+      <c r="C212" s="8"/>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="18"/>
+      <c r="C213" s="8"/>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="18"/>
+      <c r="C214" s="8"/>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="18"/>
+      <c r="C215" s="8"/>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C216" s="18"/>
+      <c r="C216" s="8"/>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C217" s="18"/>
+      <c r="C217" s="8"/>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C218" s="18"/>
+      <c r="C218" s="8"/>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="18"/>
+      <c r="C219" s="8"/>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C220" s="18"/>
+      <c r="C220" s="8"/>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="18"/>
+      <c r="C221" s="8"/>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="18"/>
+      <c r="C222" s="8"/>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="18"/>
+      <c r="C223" s="8"/>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="18"/>
+      <c r="C224" s="8"/>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C225" s="18"/>
+      <c r="C225" s="8"/>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="18"/>
+      <c r="C226" s="8"/>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="18"/>
+      <c r="C227" s="8"/>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C228" s="18"/>
+      <c r="C228" s="8"/>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C229" s="18"/>
+      <c r="C229" s="8"/>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C230" s="18"/>
+      <c r="C230" s="8"/>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C231" s="18"/>
+      <c r="C231" s="8"/>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C232" s="18"/>
+      <c r="C232" s="8"/>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C233" s="18"/>
+      <c r="C233" s="8"/>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="18"/>
+      <c r="C234" s="8"/>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="18"/>
+      <c r="C235" s="8"/>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C236" s="18"/>
+      <c r="C236" s="8"/>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C237" s="18"/>
+      <c r="C237" s="8"/>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C238" s="18"/>
+      <c r="C238" s="8"/>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C239" s="18"/>
+      <c r="C239" s="8"/>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C240" s="18"/>
+      <c r="C240" s="8"/>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C241" s="18"/>
+      <c r="C241" s="8"/>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C242" s="18"/>
+      <c r="C242" s="8"/>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C243" s="18"/>
+      <c r="C243" s="8"/>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C244" s="18"/>
+      <c r="C244" s="8"/>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C245" s="18"/>
+      <c r="C245" s="8"/>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C246" s="18"/>
+      <c r="C246" s="8"/>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C247" s="18"/>
+      <c r="C247" s="8"/>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C248" s="18"/>
+      <c r="C248" s="8"/>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C249" s="18"/>
+      <c r="C249" s="8"/>
     </row>
     <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C250" s="18"/>
+      <c r="C250" s="8"/>
     </row>
     <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C251" s="18"/>
+      <c r="C251" s="8"/>
     </row>
     <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C252" s="18"/>
+      <c r="C252" s="8"/>
     </row>
     <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="18"/>
+      <c r="C253" s="8"/>
     </row>
     <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C254" s="18"/>
+      <c r="C254" s="8"/>
     </row>
     <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C255" s="18"/>
+      <c r="C255" s="8"/>
     </row>
     <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C256" s="18"/>
+      <c r="C256" s="8"/>
     </row>
     <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C257" s="18"/>
+      <c r="C257" s="8"/>
     </row>
     <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C258" s="18"/>
+      <c r="C258" s="8"/>
     </row>
     <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C259" s="18"/>
+      <c r="C259" s="8"/>
     </row>
     <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C260" s="18"/>
+      <c r="C260" s="8"/>
     </row>
     <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C261" s="18"/>
+      <c r="C261" s="8"/>
     </row>
     <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C262" s="18"/>
+      <c r="C262" s="8"/>
     </row>
     <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C263" s="18"/>
+      <c r="C263" s="8"/>
     </row>
     <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C264" s="18"/>
+      <c r="C264" s="8"/>
     </row>
     <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C265" s="18"/>
+      <c r="C265" s="8"/>
     </row>
     <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C266" s="18"/>
+      <c r="C266" s="8"/>
     </row>
     <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C267" s="18"/>
+      <c r="C267" s="8"/>
     </row>
     <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C268" s="18"/>
+      <c r="C268" s="8"/>
     </row>
     <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C269" s="18"/>
+      <c r="C269" s="8"/>
     </row>
     <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C270" s="18"/>
+      <c r="C270" s="8"/>
     </row>
     <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C271" s="18"/>
+      <c r="C271" s="8"/>
     </row>
     <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C272" s="18"/>
+      <c r="C272" s="8"/>
     </row>
     <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C273" s="18"/>
+      <c r="C273" s="8"/>
     </row>
     <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C274" s="18"/>
+      <c r="C274" s="8"/>
     </row>
     <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C275" s="18"/>
+      <c r="C275" s="8"/>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C276" s="18"/>
+      <c r="C276" s="8"/>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C277" s="18"/>
+      <c r="C277" s="8"/>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C278" s="18"/>
+      <c r="C278" s="8"/>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C279" s="18"/>
+      <c r="C279" s="8"/>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C280" s="18"/>
+      <c r="C280" s="8"/>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C281" s="18"/>
+      <c r="C281" s="8"/>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C282" s="18"/>
+      <c r="C282" s="8"/>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C283" s="18"/>
+      <c r="C283" s="8"/>
     </row>
     <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C284" s="18"/>
+      <c r="C284" s="8"/>
     </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C285" s="18"/>
+      <c r="C285" s="8"/>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C286" s="18"/>
+      <c r="C286" s="8"/>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C287" s="18"/>
+      <c r="C287" s="8"/>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C288" s="18"/>
+      <c r="C288" s="8"/>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C289" s="18"/>
+      <c r="C289" s="8"/>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C290" s="18"/>
+      <c r="C290" s="8"/>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C291" s="18"/>
+      <c r="C291" s="8"/>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C292" s="18"/>
+      <c r="C292" s="8"/>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C293" s="18"/>
+      <c r="C293" s="8"/>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C294" s="18"/>
+      <c r="C294" s="8"/>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C295" s="18"/>
+      <c r="C295" s="8"/>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C296" s="18"/>
+      <c r="C296" s="8"/>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C297" s="18"/>
+      <c r="C297" s="8"/>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="18"/>
+      <c r="C298" s="8"/>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C299" s="18"/>
+      <c r="C299" s="8"/>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C300" s="18"/>
+      <c r="C300" s="8"/>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C301" s="18"/>
+      <c r="C301" s="8"/>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C302" s="18"/>
+      <c r="C302" s="8"/>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C303" s="18"/>
+      <c r="C303" s="8"/>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C304" s="18"/>
+      <c r="C304" s="8"/>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C305" s="18"/>
+      <c r="C305" s="8"/>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C306" s="18"/>
+      <c r="C306" s="8"/>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C307" s="18"/>
+      <c r="C307" s="8"/>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C308" s="18"/>
+      <c r="C308" s="8"/>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C309" s="18"/>
+      <c r="C309" s="8"/>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C310" s="18"/>
+      <c r="C310" s="8"/>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C311" s="18"/>
+      <c r="C311" s="8"/>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C312" s="18"/>
+      <c r="C312" s="8"/>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C313" s="18"/>
+      <c r="C313" s="8"/>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C314" s="18"/>
+      <c r="C314" s="8"/>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C315" s="18"/>
+      <c r="C315" s="8"/>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C316" s="18"/>
+      <c r="C316" s="8"/>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C317" s="18"/>
+      <c r="C317" s="8"/>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C318" s="18"/>
+      <c r="C318" s="8"/>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C319" s="18"/>
+      <c r="C319" s="8"/>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C320" s="18"/>
+      <c r="C320" s="8"/>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C321" s="18"/>
+      <c r="C321" s="8"/>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C322" s="18"/>
+      <c r="C322" s="8"/>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C323" s="18"/>
+      <c r="C323" s="8"/>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C324" s="18"/>
+      <c r="C324" s="8"/>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C325" s="18"/>
+      <c r="C325" s="8"/>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C326" s="18"/>
+      <c r="C326" s="8"/>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C327" s="18"/>
+      <c r="C327" s="8"/>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C328" s="18"/>
+      <c r="C328" s="8"/>
     </row>
     <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C329" s="18"/>
+      <c r="C329" s="8"/>
     </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C330" s="18"/>
+      <c r="C330" s="8"/>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C331" s="18"/>
+      <c r="C331" s="8"/>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C332" s="18"/>
+      <c r="C332" s="8"/>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C333" s="18"/>
+      <c r="C333" s="8"/>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C334" s="18"/>
+      <c r="C334" s="8"/>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C335" s="18"/>
+      <c r="C335" s="8"/>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C336" s="18"/>
+      <c r="C336" s="8"/>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C337" s="18"/>
+      <c r="C337" s="8"/>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C338" s="18"/>
+      <c r="C338" s="8"/>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C339" s="18"/>
+      <c r="C339" s="8"/>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C340" s="18"/>
+      <c r="C340" s="8"/>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C341" s="18"/>
+      <c r="C341" s="8"/>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C342" s="18"/>
+      <c r="C342" s="8"/>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C343" s="18"/>
+      <c r="C343" s="8"/>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C344" s="18"/>
+      <c r="C344" s="8"/>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C345" s="18"/>
+      <c r="C345" s="8"/>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C346" s="18"/>
+      <c r="C346" s="8"/>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C347" s="18"/>
+      <c r="C347" s="8"/>
     </row>
     <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C348" s="18"/>
+      <c r="C348" s="8"/>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C349" s="18"/>
+      <c r="C349" s="8"/>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C350" s="18"/>
+      <c r="C350" s="8"/>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C351" s="18"/>
+      <c r="C351" s="8"/>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C352" s="18"/>
+      <c r="C352" s="8"/>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C353" s="18"/>
+      <c r="C353" s="8"/>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C354" s="18"/>
+      <c r="C354" s="8"/>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C355" s="18"/>
+      <c r="C355" s="8"/>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C356" s="18"/>
+      <c r="C356" s="8"/>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C357" s="18"/>
+      <c r="C357" s="8"/>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C358" s="18"/>
+      <c r="C358" s="8"/>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C359" s="18"/>
+      <c r="C359" s="8"/>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C360" s="18"/>
+      <c r="C360" s="8"/>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C361" s="18"/>
+      <c r="C361" s="8"/>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C362" s="18"/>
+      <c r="C362" s="8"/>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C363" s="18"/>
+      <c r="C363" s="8"/>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C364" s="18"/>
+      <c r="C364" s="8"/>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C365" s="18"/>
+      <c r="C365" s="8"/>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C366" s="18"/>
+      <c r="C366" s="8"/>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C367" s="18"/>
+      <c r="C367" s="8"/>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C368" s="18"/>
+      <c r="C368" s="8"/>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C369" s="18"/>
+      <c r="C369" s="8"/>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C370" s="18"/>
+      <c r="C370" s="8"/>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C371" s="18"/>
+      <c r="C371" s="8"/>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C372" s="18"/>
+      <c r="C372" s="8"/>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C373" s="18"/>
+      <c r="C373" s="8"/>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C374" s="18"/>
+      <c r="C374" s="8"/>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C375" s="18"/>
+      <c r="C375" s="8"/>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C376" s="18"/>
+      <c r="C376" s="8"/>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C377" s="18"/>
+      <c r="C377" s="8"/>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C378" s="18"/>
+      <c r="C378" s="8"/>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C379" s="18"/>
+      <c r="C379" s="8"/>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C380" s="18"/>
+      <c r="C380" s="8"/>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C381" s="18"/>
+      <c r="C381" s="8"/>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C382" s="18"/>
+      <c r="C382" s="8"/>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C383" s="18"/>
+      <c r="C383" s="8"/>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C384" s="18"/>
+      <c r="C384" s="8"/>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C385" s="18"/>
+      <c r="C385" s="8"/>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C386" s="18"/>
+      <c r="C386" s="8"/>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C387" s="18"/>
+      <c r="C387" s="8"/>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C388" s="18"/>
+      <c r="C388" s="8"/>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C389" s="18"/>
+      <c r="C389" s="8"/>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C390" s="18"/>
+      <c r="C390" s="8"/>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C391" s="18"/>
+      <c r="C391" s="8"/>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C392" s="18"/>
+      <c r="C392" s="8"/>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C393" s="18"/>
+      <c r="C393" s="8"/>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C394" s="18"/>
+      <c r="C394" s="8"/>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C395" s="18"/>
+      <c r="C395" s="8"/>
     </row>
     <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C396" s="18"/>
+      <c r="C396" s="8"/>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C397" s="18"/>
+      <c r="C397" s="8"/>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C398" s="18"/>
+      <c r="C398" s="8"/>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C399" s="18"/>
+      <c r="C399" s="8"/>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C400" s="18"/>
+      <c r="C400" s="8"/>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C401" s="18"/>
+      <c r="C401" s="8"/>
     </row>
     <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C402" s="18"/>
+      <c r="C402" s="8"/>
     </row>
     <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C403" s="18"/>
+      <c r="C403" s="8"/>
     </row>
     <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C404" s="18"/>
+      <c r="C404" s="8"/>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C405" s="18"/>
+      <c r="C405" s="8"/>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C406" s="18"/>
+      <c r="C406" s="8"/>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C407" s="18"/>
+      <c r="C407" s="8"/>
     </row>
     <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C408" s="18"/>
+      <c r="C408" s="8"/>
     </row>
     <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C409" s="18"/>
+      <c r="C409" s="8"/>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C410" s="18"/>
+      <c r="C410" s="8"/>
     </row>
     <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C411" s="18"/>
+      <c r="C411" s="8"/>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C412" s="18"/>
+      <c r="C412" s="8"/>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C413" s="18"/>
+      <c r="C413" s="8"/>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C414" s="18"/>
+      <c r="C414" s="8"/>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C415" s="18"/>
+      <c r="C415" s="8"/>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C416" s="18"/>
+      <c r="C416" s="8"/>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C417" s="18"/>
+      <c r="C417" s="8"/>
     </row>
     <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C418" s="18"/>
+      <c r="C418" s="8"/>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C419" s="18"/>
+      <c r="C419" s="8"/>
     </row>
     <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C420" s="18"/>
+      <c r="C420" s="8"/>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C421" s="18"/>
+      <c r="C421" s="8"/>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C422" s="18"/>
+      <c r="C422" s="8"/>
     </row>
     <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C423" s="18"/>
+      <c r="C423" s="8"/>
     </row>
     <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C424" s="18"/>
+      <c r="C424" s="8"/>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C425" s="18"/>
+      <c r="C425" s="8"/>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C426" s="18"/>
+      <c r="C426" s="8"/>
     </row>
     <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C427" s="18"/>
+      <c r="C427" s="8"/>
     </row>
     <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C428" s="18"/>
+      <c r="C428" s="8"/>
     </row>
     <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C429" s="18"/>
+      <c r="C429" s="8"/>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C430" s="18"/>
+      <c r="C430" s="8"/>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C431" s="18"/>
+      <c r="C431" s="8"/>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C432" s="18"/>
+      <c r="C432" s="8"/>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C433" s="18"/>
+      <c r="C433" s="8"/>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C434" s="18"/>
+      <c r="C434" s="8"/>
     </row>
     <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C435" s="18"/>
+      <c r="C435" s="8"/>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C436" s="18"/>
+      <c r="C436" s="8"/>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C437" s="18"/>
+      <c r="C437" s="8"/>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C438" s="18"/>
+      <c r="C438" s="8"/>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C439" s="18"/>
+      <c r="C439" s="8"/>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C440" s="18"/>
+      <c r="C440" s="8"/>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C441" s="18"/>
+      <c r="C441" s="8"/>
     </row>
     <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C442" s="18"/>
+      <c r="C442" s="8"/>
     </row>
     <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C443" s="18"/>
+      <c r="C443" s="8"/>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C444" s="18"/>
+      <c r="C444" s="8"/>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C445" s="18"/>
+      <c r="C445" s="8"/>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C446" s="18"/>
+      <c r="C446" s="8"/>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C447" s="18"/>
+      <c r="C447" s="8"/>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C448" s="18"/>
+      <c r="C448" s="8"/>
     </row>
     <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C449" s="18"/>
+      <c r="C449" s="8"/>
     </row>
     <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C450" s="18"/>
+      <c r="C450" s="8"/>
     </row>
     <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C451" s="18"/>
+      <c r="C451" s="8"/>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C452" s="18"/>
+      <c r="C452" s="8"/>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C453" s="18"/>
+      <c r="C453" s="8"/>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C454" s="18"/>
+      <c r="C454" s="8"/>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C455" s="18"/>
+      <c r="C455" s="8"/>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C456" s="18"/>
+      <c r="C456" s="8"/>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C457" s="18"/>
+      <c r="C457" s="8"/>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C458" s="18"/>
+      <c r="C458" s="8"/>
     </row>
     <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C459" s="18"/>
+      <c r="C459" s="8"/>
     </row>
     <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C460" s="18"/>
+      <c r="C460" s="8"/>
     </row>
     <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C461" s="18"/>
+      <c r="C461" s="8"/>
     </row>
     <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C462" s="18"/>
+      <c r="C462" s="8"/>
     </row>
     <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C463" s="18"/>
+      <c r="C463" s="8"/>
     </row>
     <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C464" s="18"/>
+      <c r="C464" s="8"/>
     </row>
     <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C465" s="18"/>
+      <c r="C465" s="8"/>
     </row>
     <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C466" s="18"/>
+      <c r="C466" s="8"/>
     </row>
     <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C467" s="18"/>
+      <c r="C467" s="8"/>
     </row>
     <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C468" s="18"/>
+      <c r="C468" s="8"/>
     </row>
     <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C469" s="18"/>
+      <c r="C469" s="8"/>
     </row>
     <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C470" s="18"/>
+      <c r="C470" s="8"/>
     </row>
     <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C471" s="18"/>
+      <c r="C471" s="8"/>
     </row>
     <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C472" s="18"/>
+      <c r="C472" s="8"/>
     </row>
     <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C473" s="18"/>
+      <c r="C473" s="8"/>
     </row>
     <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C474" s="18"/>
+      <c r="C474" s="8"/>
     </row>
     <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C475" s="18"/>
+      <c r="C475" s="8"/>
     </row>
     <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C476" s="18"/>
+      <c r="C476" s="8"/>
     </row>
     <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C477" s="18"/>
+      <c r="C477" s="8"/>
     </row>
     <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C478" s="18"/>
+      <c r="C478" s="8"/>
     </row>
     <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C479" s="18"/>
+      <c r="C479" s="8"/>
     </row>
     <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C480" s="18"/>
+      <c r="C480" s="8"/>
     </row>
     <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C481" s="18"/>
+      <c r="C481" s="8"/>
     </row>
     <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C482" s="18"/>
+      <c r="C482" s="8"/>
     </row>
     <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C483" s="18"/>
+      <c r="C483" s="8"/>
     </row>
     <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C484" s="18"/>
+      <c r="C484" s="8"/>
     </row>
     <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C485" s="18"/>
+      <c r="C485" s="8"/>
     </row>
     <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C486" s="18"/>
+      <c r="C486" s="8"/>
     </row>
     <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C487" s="18"/>
+      <c r="C487" s="8"/>
     </row>
     <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C488" s="18"/>
+      <c r="C488" s="8"/>
     </row>
     <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C489" s="18"/>
+      <c r="C489" s="8"/>
     </row>
     <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C490" s="18"/>
+      <c r="C490" s="8"/>
     </row>
     <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C491" s="18"/>
+      <c r="C491" s="8"/>
     </row>
     <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C492" s="18"/>
+      <c r="C492" s="8"/>
     </row>
     <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C493" s="18"/>
+      <c r="C493" s="8"/>
     </row>
     <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C494" s="18"/>
+      <c r="C494" s="8"/>
     </row>
     <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C495" s="18"/>
+      <c r="C495" s="8"/>
     </row>
     <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C496" s="18"/>
+      <c r="C496" s="8"/>
     </row>
     <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C497" s="18"/>
+      <c r="C497" s="8"/>
     </row>
     <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C498" s="18"/>
+      <c r="C498" s="8"/>
     </row>
     <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C499" s="18"/>
+      <c r="C499" s="8"/>
     </row>
     <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C500" s="18"/>
+      <c r="C500" s="8"/>
     </row>
     <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C501" s="18"/>
+      <c r="C501" s="8"/>
     </row>
     <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C502" s="18"/>
+      <c r="C502" s="8"/>
     </row>
     <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C503" s="18"/>
+      <c r="C503" s="8"/>
     </row>
     <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C504" s="18"/>
+      <c r="C504" s="8"/>
     </row>
     <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C505" s="18"/>
+      <c r="C505" s="8"/>
     </row>
     <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C506" s="18"/>
+      <c r="C506" s="8"/>
     </row>
     <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C507" s="18"/>
+      <c r="C507" s="8"/>
     </row>
     <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C508" s="18"/>
+      <c r="C508" s="8"/>
     </row>
     <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C509" s="18"/>
+      <c r="C509" s="8"/>
     </row>
     <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C510" s="18"/>
+      <c r="C510" s="8"/>
     </row>
     <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C511" s="18"/>
+      <c r="C511" s="8"/>
     </row>
     <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C512" s="18"/>
+      <c r="C512" s="8"/>
     </row>
     <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C513" s="18"/>
+      <c r="C513" s="8"/>
     </row>
     <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C514" s="18"/>
+      <c r="C514" s="8"/>
     </row>
     <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C515" s="18"/>
+      <c r="C515" s="8"/>
     </row>
     <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C516" s="18"/>
+      <c r="C516" s="8"/>
     </row>
     <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C517" s="18"/>
+      <c r="C517" s="8"/>
     </row>
     <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C518" s="18"/>
+      <c r="C518" s="8"/>
     </row>
     <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C519" s="18"/>
+      <c r="C519" s="8"/>
     </row>
     <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C520" s="18"/>
+      <c r="C520" s="8"/>
     </row>
     <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C521" s="18"/>
+      <c r="C521" s="8"/>
     </row>
     <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C522" s="18"/>
+      <c r="C522" s="8"/>
     </row>
     <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C523" s="18"/>
+      <c r="C523" s="8"/>
     </row>
     <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C524" s="18"/>
+      <c r="C524" s="8"/>
     </row>
     <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C525" s="18"/>
+      <c r="C525" s="8"/>
     </row>
     <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C526" s="18"/>
+      <c r="C526" s="8"/>
     </row>
     <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C527" s="18"/>
+      <c r="C527" s="8"/>
     </row>
     <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C528" s="18"/>
+      <c r="C528" s="8"/>
     </row>
     <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C529" s="18"/>
+      <c r="C529" s="8"/>
     </row>
     <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C530" s="18"/>
+      <c r="C530" s="8"/>
     </row>
     <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C531" s="18"/>
+      <c r="C531" s="8"/>
     </row>
     <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C532" s="18"/>
+      <c r="C532" s="8"/>
     </row>
     <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C533" s="18"/>
+      <c r="C533" s="8"/>
     </row>
     <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C534" s="18"/>
+      <c r="C534" s="8"/>
     </row>
     <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C535" s="18"/>
+      <c r="C535" s="8"/>
     </row>
     <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C536" s="18"/>
+      <c r="C536" s="8"/>
     </row>
     <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C537" s="18"/>
+      <c r="C537" s="8"/>
     </row>
     <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C538" s="18"/>
+      <c r="C538" s="8"/>
     </row>
     <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C539" s="18"/>
+      <c r="C539" s="8"/>
     </row>
     <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C540" s="18"/>
+      <c r="C540" s="8"/>
     </row>
     <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C541" s="18"/>
+      <c r="C541" s="8"/>
     </row>
     <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C542" s="18"/>
+      <c r="C542" s="8"/>
     </row>
     <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C543" s="18"/>
+      <c r="C543" s="8"/>
     </row>
     <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C544" s="18"/>
+      <c r="C544" s="8"/>
     </row>
     <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C545" s="18"/>
+      <c r="C545" s="8"/>
     </row>
     <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C546" s="18"/>
+      <c r="C546" s="8"/>
     </row>
     <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C547" s="18"/>
+      <c r="C547" s="8"/>
     </row>
     <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C548" s="18"/>
+      <c r="C548" s="8"/>
     </row>
     <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C549" s="18"/>
+      <c r="C549" s="8"/>
     </row>
     <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C550" s="18"/>
+      <c r="C550" s="8"/>
     </row>
     <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C551" s="18"/>
+      <c r="C551" s="8"/>
     </row>
     <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C552" s="18"/>
+      <c r="C552" s="8"/>
     </row>
     <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C553" s="18"/>
+      <c r="C553" s="8"/>
     </row>
     <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C554" s="18"/>
+      <c r="C554" s="8"/>
     </row>
     <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C555" s="18"/>
+      <c r="C555" s="8"/>
     </row>
     <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C556" s="18"/>
+      <c r="C556" s="8"/>
     </row>
     <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C557" s="18"/>
+      <c r="C557" s="8"/>
     </row>
     <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C558" s="18"/>
+      <c r="C558" s="8"/>
     </row>
     <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C559" s="18"/>
+      <c r="C559" s="8"/>
     </row>
     <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C560" s="18"/>
+      <c r="C560" s="8"/>
     </row>
     <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C561" s="18"/>
+      <c r="C561" s="8"/>
     </row>
     <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C562" s="18"/>
+      <c r="C562" s="8"/>
     </row>
     <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C563" s="18"/>
+      <c r="C563" s="8"/>
     </row>
     <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C564" s="18"/>
+      <c r="C564" s="8"/>
     </row>
     <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C565" s="18"/>
+      <c r="C565" s="8"/>
     </row>
     <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C566" s="18"/>
+      <c r="C566" s="8"/>
     </row>
     <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C567" s="18"/>
+      <c r="C567" s="8"/>
     </row>
     <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C568" s="18"/>
+      <c r="C568" s="8"/>
     </row>
     <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C569" s="18"/>
+      <c r="C569" s="8"/>
     </row>
     <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C570" s="18"/>
+      <c r="C570" s="8"/>
     </row>
     <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C571" s="18"/>
+      <c r="C571" s="8"/>
     </row>
     <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C572" s="18"/>
+      <c r="C572" s="8"/>
     </row>
     <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C573" s="18"/>
+      <c r="C573" s="8"/>
     </row>
     <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C574" s="18"/>
+      <c r="C574" s="8"/>
     </row>
     <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C575" s="18"/>
+      <c r="C575" s="8"/>
     </row>
     <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C576" s="18"/>
+      <c r="C576" s="8"/>
     </row>
     <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C577" s="18"/>
+      <c r="C577" s="8"/>
     </row>
     <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C578" s="18"/>
+      <c r="C578" s="8"/>
     </row>
     <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C579" s="18"/>
+      <c r="C579" s="8"/>
     </row>
     <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C580" s="18"/>
+      <c r="C580" s="8"/>
     </row>
     <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C581" s="18"/>
+      <c r="C581" s="8"/>
     </row>
     <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C582" s="18"/>
+      <c r="C582" s="8"/>
     </row>
     <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C583" s="18"/>
+      <c r="C583" s="8"/>
     </row>
     <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C584" s="18"/>
+      <c r="C584" s="8"/>
     </row>
     <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C585" s="18"/>
+      <c r="C585" s="8"/>
     </row>
     <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C586" s="18"/>
+      <c r="C586" s="8"/>
     </row>
     <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C587" s="18"/>
+      <c r="C587" s="8"/>
     </row>
     <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C588" s="18"/>
+      <c r="C588" s="8"/>
     </row>
     <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C589" s="18"/>
+      <c r="C589" s="8"/>
     </row>
     <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C590" s="18"/>
+      <c r="C590" s="8"/>
     </row>
     <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C591" s="18"/>
+      <c r="C591" s="8"/>
     </row>
     <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C592" s="18"/>
+      <c r="C592" s="8"/>
     </row>
     <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C593" s="18"/>
+      <c r="C593" s="8"/>
     </row>
     <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C594" s="18"/>
+      <c r="C594" s="8"/>
     </row>
     <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C595" s="18"/>
+      <c r="C595" s="8"/>
     </row>
     <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C596" s="18"/>
+      <c r="C596" s="8"/>
     </row>
     <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C597" s="18"/>
+      <c r="C597" s="8"/>
     </row>
     <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C598" s="18"/>
+      <c r="C598" s="8"/>
     </row>
     <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C599" s="18"/>
+      <c r="C599" s="8"/>
     </row>
     <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C600" s="18"/>
+      <c r="C600" s="8"/>
     </row>
     <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C601" s="18"/>
+      <c r="C601" s="8"/>
     </row>
     <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C602" s="18"/>
+      <c r="C602" s="8"/>
     </row>
     <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C603" s="18"/>
+      <c r="C603" s="8"/>
     </row>
     <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C604" s="18"/>
+      <c r="C604" s="8"/>
     </row>
     <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C605" s="18"/>
+      <c r="C605" s="8"/>
     </row>
     <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C606" s="18"/>
+      <c r="C606" s="8"/>
     </row>
     <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C607" s="18"/>
+      <c r="C607" s="8"/>
     </row>
     <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C608" s="18"/>
+      <c r="C608" s="8"/>
     </row>
     <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C609" s="18"/>
+      <c r="C609" s="8"/>
     </row>
     <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C610" s="18"/>
+      <c r="C610" s="8"/>
     </row>
     <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C611" s="18"/>
+      <c r="C611" s="8"/>
     </row>
     <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C612" s="18"/>
+      <c r="C612" s="8"/>
     </row>
     <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C613" s="18"/>
+      <c r="C613" s="8"/>
     </row>
     <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C614" s="18"/>
+      <c r="C614" s="8"/>
     </row>
     <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C615" s="18"/>
+      <c r="C615" s="8"/>
     </row>
     <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C616" s="18"/>
+      <c r="C616" s="8"/>
     </row>
     <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C617" s="18"/>
+      <c r="C617" s="8"/>
     </row>
     <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C618" s="18"/>
+      <c r="C618" s="8"/>
     </row>
     <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C619" s="18"/>
+      <c r="C619" s="8"/>
     </row>
     <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C620" s="18"/>
+      <c r="C620" s="8"/>
     </row>
     <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C621" s="18"/>
+      <c r="C621" s="8"/>
     </row>
     <row r="622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C622" s="18"/>
+      <c r="C622" s="8"/>
     </row>
     <row r="623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C623" s="18"/>
+      <c r="C623" s="8"/>
     </row>
     <row r="624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C624" s="18"/>
+      <c r="C624" s="8"/>
     </row>
     <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C625" s="18"/>
+      <c r="C625" s="8"/>
     </row>
     <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C626" s="18"/>
+      <c r="C626" s="8"/>
     </row>
     <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C627" s="18"/>
+      <c r="C627" s="8"/>
     </row>
     <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C628" s="18"/>
+      <c r="C628" s="8"/>
     </row>
     <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C629" s="18"/>
+      <c r="C629" s="8"/>
     </row>
     <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C630" s="18"/>
+      <c r="C630" s="8"/>
     </row>
     <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C631" s="18"/>
+      <c r="C631" s="8"/>
     </row>
     <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C632" s="18"/>
+      <c r="C632" s="8"/>
     </row>
     <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C633" s="18"/>
+      <c r="C633" s="8"/>
     </row>
     <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C634" s="18"/>
+      <c r="C634" s="8"/>
     </row>
     <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C635" s="18"/>
+      <c r="C635" s="8"/>
     </row>
     <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C636" s="18"/>
+      <c r="C636" s="8"/>
     </row>
     <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C637" s="18"/>
+      <c r="C637" s="8"/>
     </row>
     <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C638" s="18"/>
+      <c r="C638" s="8"/>
     </row>
     <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C639" s="18"/>
+      <c r="C639" s="8"/>
     </row>
     <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C640" s="18"/>
+      <c r="C640" s="8"/>
     </row>
     <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C641" s="18"/>
+      <c r="C641" s="8"/>
     </row>
     <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C642" s="18"/>
+      <c r="C642" s="8"/>
     </row>
     <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C643" s="18"/>
+      <c r="C643" s="8"/>
     </row>
     <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C644" s="18"/>
+      <c r="C644" s="8"/>
     </row>
     <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C645" s="18"/>
+      <c r="C645" s="8"/>
     </row>
     <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C646" s="18"/>
+      <c r="C646" s="8"/>
     </row>
     <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C647" s="18"/>
+      <c r="C647" s="8"/>
     </row>
     <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C648" s="18"/>
+      <c r="C648" s="8"/>
     </row>
     <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C649" s="18"/>
+      <c r="C649" s="8"/>
     </row>
     <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C650" s="18"/>
+      <c r="C650" s="8"/>
     </row>
     <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C651" s="18"/>
+      <c r="C651" s="8"/>
     </row>
     <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C652" s="18"/>
+      <c r="C652" s="8"/>
     </row>
     <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C653" s="18"/>
+      <c r="C653" s="8"/>
     </row>
     <row r="654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C654" s="18"/>
+      <c r="C654" s="8"/>
     </row>
     <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C655" s="18"/>
+      <c r="C655" s="8"/>
     </row>
     <row r="656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C656" s="18"/>
+      <c r="C656" s="8"/>
     </row>
     <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C657" s="18"/>
+      <c r="C657" s="8"/>
     </row>
     <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C658" s="18"/>
+      <c r="C658" s="8"/>
     </row>
     <row r="659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C659" s="18"/>
+      <c r="C659" s="8"/>
     </row>
     <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C660" s="18"/>
+      <c r="C660" s="8"/>
     </row>
     <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C661" s="18"/>
+      <c r="C661" s="8"/>
     </row>
     <row r="662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C662" s="18"/>
+      <c r="C662" s="8"/>
     </row>
     <row r="663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C663" s="18"/>
+      <c r="C663" s="8"/>
     </row>
     <row r="664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C664" s="18"/>
+      <c r="C664" s="8"/>
     </row>
     <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C665" s="18"/>
+      <c r="C665" s="8"/>
     </row>
     <row r="666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C666" s="18"/>
+      <c r="C666" s="8"/>
     </row>
     <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C667" s="18"/>
+      <c r="C667" s="8"/>
     </row>
     <row r="668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C668" s="18"/>
+      <c r="C668" s="8"/>
     </row>
     <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C669" s="18"/>
+      <c r="C669" s="8"/>
     </row>
     <row r="670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C670" s="18"/>
+      <c r="C670" s="8"/>
     </row>
     <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C671" s="18"/>
+      <c r="C671" s="8"/>
     </row>
     <row r="672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C672" s="18"/>
+      <c r="C672" s="8"/>
     </row>
     <row r="673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C673" s="18"/>
+      <c r="C673" s="8"/>
     </row>
     <row r="674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C674" s="18"/>
+      <c r="C674" s="8"/>
     </row>
     <row r="675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C675" s="18"/>
+      <c r="C675" s="8"/>
     </row>
     <row r="676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C676" s="18"/>
+      <c r="C676" s="8"/>
     </row>
     <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C677" s="18"/>
+      <c r="C677" s="8"/>
     </row>
     <row r="678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C678" s="18"/>
+      <c r="C678" s="8"/>
     </row>
     <row r="679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C679" s="18"/>
+      <c r="C679" s="8"/>
     </row>
     <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C680" s="18"/>
+      <c r="C680" s="8"/>
     </row>
     <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C681" s="18"/>
+      <c r="C681" s="8"/>
     </row>
     <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C682" s="18"/>
+      <c r="C682" s="8"/>
     </row>
     <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C683" s="18"/>
+      <c r="C683" s="8"/>
     </row>
     <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C684" s="18"/>
+      <c r="C684" s="8"/>
     </row>
     <row r="685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C685" s="18"/>
+      <c r="C685" s="8"/>
     </row>
     <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C686" s="18"/>
+      <c r="C686" s="8"/>
     </row>
     <row r="687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C687" s="18"/>
+      <c r="C687" s="8"/>
     </row>
     <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C688" s="18"/>
+      <c r="C688" s="8"/>
     </row>
     <row r="689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C689" s="18"/>
+      <c r="C689" s="8"/>
     </row>
     <row r="690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C690" s="18"/>
+      <c r="C690" s="8"/>
     </row>
     <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C691" s="18"/>
+      <c r="C691" s="8"/>
     </row>
     <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C692" s="18"/>
+      <c r="C692" s="8"/>
     </row>
     <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C693" s="18"/>
+      <c r="C693" s="8"/>
     </row>
     <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C694" s="18"/>
+      <c r="C694" s="8"/>
     </row>
     <row r="695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C695" s="18"/>
+      <c r="C695" s="8"/>
     </row>
     <row r="696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C696" s="18"/>
+      <c r="C696" s="8"/>
     </row>
     <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C697" s="18"/>
+      <c r="C697" s="8"/>
     </row>
     <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C698" s="18"/>
+      <c r="C698" s="8"/>
     </row>
     <row r="699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C699" s="18"/>
+      <c r="C699" s="8"/>
     </row>
     <row r="700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C700" s="18"/>
+      <c r="C700" s="8"/>
     </row>
     <row r="701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C701" s="18"/>
+      <c r="C701" s="8"/>
     </row>
     <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C702" s="18"/>
+      <c r="C702" s="8"/>
     </row>
     <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C703" s="18"/>
+      <c r="C703" s="8"/>
     </row>
     <row r="704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C704" s="18"/>
+      <c r="C704" s="8"/>
     </row>
     <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C705" s="18"/>
+      <c r="C705" s="8"/>
     </row>
     <row r="706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C706" s="18"/>
+      <c r="C706" s="8"/>
     </row>
     <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C707" s="18"/>
+      <c r="C707" s="8"/>
     </row>
     <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C708" s="18"/>
+      <c r="C708" s="8"/>
     </row>
     <row r="709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C709" s="18"/>
+      <c r="C709" s="8"/>
     </row>
     <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C710" s="18"/>
+      <c r="C710" s="8"/>
     </row>
     <row r="711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C711" s="18"/>
+      <c r="C711" s="8"/>
     </row>
     <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C712" s="18"/>
+      <c r="C712" s="8"/>
     </row>
     <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C713" s="18"/>
+      <c r="C713" s="8"/>
     </row>
     <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C714" s="18"/>
+      <c r="C714" s="8"/>
     </row>
     <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C715" s="18"/>
+      <c r="C715" s="8"/>
     </row>
     <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C716" s="18"/>
+      <c r="C716" s="8"/>
     </row>
     <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C717" s="18"/>
+      <c r="C717" s="8"/>
     </row>
     <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C718" s="18"/>
+      <c r="C718" s="8"/>
     </row>
     <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C719" s="18"/>
+      <c r="C719" s="8"/>
     </row>
     <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C720" s="18"/>
+      <c r="C720" s="8"/>
     </row>
     <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C721" s="18"/>
+      <c r="C721" s="8"/>
     </row>
     <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C722" s="18"/>
+      <c r="C722" s="8"/>
     </row>
     <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C723" s="18"/>
+      <c r="C723" s="8"/>
     </row>
     <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C724" s="18"/>
+      <c r="C724" s="8"/>
     </row>
     <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C725" s="18"/>
+      <c r="C725" s="8"/>
     </row>
     <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C726" s="18"/>
+      <c r="C726" s="8"/>
     </row>
     <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C727" s="18"/>
+      <c r="C727" s="8"/>
     </row>
     <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C728" s="18"/>
+      <c r="C728" s="8"/>
     </row>
     <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C729" s="18"/>
+      <c r="C729" s="8"/>
     </row>
     <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C730" s="18"/>
+      <c r="C730" s="8"/>
     </row>
     <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C731" s="18"/>
+      <c r="C731" s="8"/>
     </row>
     <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C732" s="18"/>
+      <c r="C732" s="8"/>
     </row>
     <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C733" s="18"/>
+      <c r="C733" s="8"/>
     </row>
     <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C734" s="18"/>
+      <c r="C734" s="8"/>
     </row>
     <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C735" s="18"/>
+      <c r="C735" s="8"/>
     </row>
     <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C736" s="18"/>
+      <c r="C736" s="8"/>
     </row>
     <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C737" s="18"/>
+      <c r="C737" s="8"/>
     </row>
     <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C738" s="18"/>
+      <c r="C738" s="8"/>
     </row>
     <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C739" s="18"/>
+      <c r="C739" s="8"/>
     </row>
     <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C740" s="18"/>
+      <c r="C740" s="8"/>
     </row>
     <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C741" s="18"/>
+      <c r="C741" s="8"/>
     </row>
     <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C742" s="18"/>
+      <c r="C742" s="8"/>
     </row>
     <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C743" s="18"/>
+      <c r="C743" s="8"/>
     </row>
     <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C744" s="18"/>
+      <c r="C744" s="8"/>
     </row>
     <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C745" s="18"/>
+      <c r="C745" s="8"/>
     </row>
     <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C746" s="18"/>
+      <c r="C746" s="8"/>
     </row>
     <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C747" s="18"/>
+      <c r="C747" s="8"/>
     </row>
     <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C748" s="18"/>
+      <c r="C748" s="8"/>
     </row>
     <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C749" s="18"/>
+      <c r="C749" s="8"/>
     </row>
     <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C750" s="18"/>
+      <c r="C750" s="8"/>
     </row>
     <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C751" s="18"/>
+      <c r="C751" s="8"/>
     </row>
     <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C752" s="18"/>
+      <c r="C752" s="8"/>
     </row>
     <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C753" s="18"/>
+      <c r="C753" s="8"/>
     </row>
     <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C754" s="18"/>
+      <c r="C754" s="8"/>
     </row>
     <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C755" s="18"/>
+      <c r="C755" s="8"/>
     </row>
     <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C756" s="18"/>
+      <c r="C756" s="8"/>
     </row>
     <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C757" s="18"/>
+      <c r="C757" s="8"/>
     </row>
     <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C758" s="18"/>
+      <c r="C758" s="8"/>
     </row>
     <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C759" s="18"/>
+      <c r="C759" s="8"/>
     </row>
     <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C760" s="18"/>
+      <c r="C760" s="8"/>
     </row>
     <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C761" s="18"/>
+      <c r="C761" s="8"/>
     </row>
     <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C762" s="18"/>
+      <c r="C762" s="8"/>
     </row>
     <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C763" s="18"/>
+      <c r="C763" s="8"/>
     </row>
     <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C764" s="18"/>
+      <c r="C764" s="8"/>
     </row>
     <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C765" s="18"/>
+      <c r="C765" s="8"/>
     </row>
     <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C766" s="18"/>
+      <c r="C766" s="8"/>
     </row>
     <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C767" s="18"/>
+      <c r="C767" s="8"/>
     </row>
     <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C768" s="18"/>
+      <c r="C768" s="8"/>
     </row>
     <row r="769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C769" s="18"/>
+      <c r="C769" s="8"/>
     </row>
     <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C770" s="18"/>
+      <c r="C770" s="8"/>
     </row>
     <row r="771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C771" s="18"/>
+      <c r="C771" s="8"/>
     </row>
     <row r="772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C772" s="18"/>
+      <c r="C772" s="8"/>
     </row>
     <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C773" s="18"/>
+      <c r="C773" s="8"/>
     </row>
     <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C774" s="18"/>
+      <c r="C774" s="8"/>
     </row>
     <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C775" s="18"/>
+      <c r="C775" s="8"/>
     </row>
     <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C776" s="18"/>
+      <c r="C776" s="8"/>
     </row>
     <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C777" s="18"/>
+      <c r="C777" s="8"/>
     </row>
     <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C778" s="18"/>
+      <c r="C778" s="8"/>
     </row>
     <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C779" s="18"/>
+      <c r="C779" s="8"/>
     </row>
     <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C780" s="18"/>
+      <c r="C780" s="8"/>
     </row>
     <row r="781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C781" s="18"/>
+      <c r="C781" s="8"/>
     </row>
     <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C782" s="18"/>
+      <c r="C782" s="8"/>
     </row>
     <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C783" s="18"/>
+      <c r="C783" s="8"/>
     </row>
     <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C784" s="18"/>
+      <c r="C784" s="8"/>
     </row>
     <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C785" s="18"/>
+      <c r="C785" s="8"/>
     </row>
     <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C786" s="18"/>
+      <c r="C786" s="8"/>
     </row>
     <row r="787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C787" s="18"/>
+      <c r="C787" s="8"/>
     </row>
     <row r="788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C788" s="18"/>
+      <c r="C788" s="8"/>
     </row>
     <row r="789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C789" s="18"/>
+      <c r="C789" s="8"/>
     </row>
     <row r="790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C790" s="18"/>
+      <c r="C790" s="8"/>
     </row>
     <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C791" s="18"/>
+      <c r="C791" s="8"/>
     </row>
     <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C792" s="18"/>
+      <c r="C792" s="8"/>
     </row>
     <row r="793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C793" s="18"/>
+      <c r="C793" s="8"/>
     </row>
     <row r="794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C794" s="18"/>
+      <c r="C794" s="8"/>
     </row>
     <row r="795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C795" s="18"/>
+      <c r="C795" s="8"/>
     </row>
     <row r="796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C796" s="18"/>
+      <c r="C796" s="8"/>
     </row>
     <row r="797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C797" s="18"/>
+      <c r="C797" s="8"/>
     </row>
     <row r="798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C798" s="18"/>
+      <c r="C798" s="8"/>
     </row>
     <row r="799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C799" s="18"/>
+      <c r="C799" s="8"/>
     </row>
     <row r="800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C800" s="18"/>
+      <c r="C800" s="8"/>
     </row>
     <row r="801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C801" s="18"/>
+      <c r="C801" s="8"/>
     </row>
     <row r="802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C802" s="18"/>
+      <c r="C802" s="8"/>
     </row>
     <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C803" s="18"/>
+      <c r="C803" s="8"/>
     </row>
     <row r="804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C804" s="18"/>
+      <c r="C804" s="8"/>
     </row>
     <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C805" s="18"/>
+      <c r="C805" s="8"/>
     </row>
     <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C806" s="18"/>
+      <c r="C806" s="8"/>
     </row>
     <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C807" s="18"/>
+      <c r="C807" s="8"/>
     </row>
     <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C808" s="18"/>
+      <c r="C808" s="8"/>
     </row>
     <row r="809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C809" s="18"/>
+      <c r="C809" s="8"/>
     </row>
     <row r="810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C810" s="18"/>
+      <c r="C810" s="8"/>
     </row>
     <row r="811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C811" s="18"/>
+      <c r="C811" s="8"/>
     </row>
     <row r="812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C812" s="18"/>
+      <c r="C812" s="8"/>
     </row>
     <row r="813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C813" s="18"/>
+      <c r="C813" s="8"/>
     </row>
     <row r="814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C814" s="18"/>
+      <c r="C814" s="8"/>
     </row>
     <row r="815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C815" s="18"/>
+      <c r="C815" s="8"/>
     </row>
     <row r="816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C816" s="18"/>
+      <c r="C816" s="8"/>
     </row>
     <row r="817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C817" s="18"/>
+      <c r="C817" s="8"/>
     </row>
     <row r="818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C818" s="18"/>
+      <c r="C818" s="8"/>
     </row>
     <row r="819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C819" s="18"/>
+      <c r="C819" s="8"/>
     </row>
     <row r="820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C820" s="18"/>
+      <c r="C820" s="8"/>
     </row>
     <row r="821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C821" s="18"/>
+      <c r="C821" s="8"/>
     </row>
     <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C822" s="18"/>
+      <c r="C822" s="8"/>
     </row>
     <row r="823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C823" s="18"/>
+      <c r="C823" s="8"/>
     </row>
     <row r="824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C824" s="18"/>
+      <c r="C824" s="8"/>
     </row>
     <row r="825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C825" s="18"/>
+      <c r="C825" s="8"/>
     </row>
     <row r="826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C826" s="18"/>
+      <c r="C826" s="8"/>
     </row>
     <row r="827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C827" s="18"/>
+      <c r="C827" s="8"/>
     </row>
     <row r="828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C828" s="18"/>
+      <c r="C828" s="8"/>
     </row>
     <row r="829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C829" s="18"/>
+      <c r="C829" s="8"/>
     </row>
     <row r="830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C830" s="18"/>
+      <c r="C830" s="8"/>
     </row>
     <row r="831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C831" s="18"/>
+      <c r="C831" s="8"/>
     </row>
     <row r="832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C832" s="18"/>
+      <c r="C832" s="8"/>
     </row>
     <row r="833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C833" s="18"/>
+      <c r="C833" s="8"/>
     </row>
     <row r="834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C834" s="18"/>
+      <c r="C834" s="8"/>
     </row>
     <row r="835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C835" s="18"/>
+      <c r="C835" s="8"/>
     </row>
     <row r="836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C836" s="18"/>
+      <c r="C836" s="8"/>
     </row>
     <row r="837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C837" s="18"/>
+      <c r="C837" s="8"/>
     </row>
     <row r="838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C838" s="18"/>
+      <c r="C838" s="8"/>
     </row>
     <row r="839" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C839" s="18"/>
+      <c r="C839" s="8"/>
     </row>
     <row r="840" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C840" s="18"/>
+      <c r="C840" s="8"/>
     </row>
     <row r="841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C841" s="18"/>
+      <c r="C841" s="8"/>
     </row>
     <row r="842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C842" s="18"/>
+      <c r="C842" s="8"/>
     </row>
     <row r="843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C843" s="18"/>
+      <c r="C843" s="8"/>
     </row>
     <row r="844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C844" s="18"/>
+      <c r="C844" s="8"/>
     </row>
     <row r="845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C845" s="18"/>
+      <c r="C845" s="8"/>
     </row>
     <row r="846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C846" s="18"/>
+      <c r="C846" s="8"/>
     </row>
     <row r="847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C847" s="18"/>
+      <c r="C847" s="8"/>
     </row>
     <row r="848" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C848" s="18"/>
+      <c r="C848" s="8"/>
     </row>
     <row r="849" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C849" s="18"/>
+      <c r="C849" s="8"/>
     </row>
     <row r="850" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C850" s="18"/>
+      <c r="C850" s="8"/>
     </row>
     <row r="851" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C851" s="18"/>
+      <c r="C851" s="8"/>
     </row>
     <row r="852" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C852" s="18"/>
+      <c r="C852" s="8"/>
     </row>
     <row r="853" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C853" s="18"/>
+      <c r="C853" s="8"/>
     </row>
     <row r="854" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C854" s="18"/>
+      <c r="C854" s="8"/>
     </row>
     <row r="855" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C855" s="18"/>
+      <c r="C855" s="8"/>
     </row>
     <row r="856" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C856" s="18"/>
+      <c r="C856" s="8"/>
     </row>
     <row r="857" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C857" s="18"/>
+      <c r="C857" s="8"/>
     </row>
     <row r="858" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C858" s="18"/>
+      <c r="C858" s="8"/>
     </row>
     <row r="859" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C859" s="18"/>
+      <c r="C859" s="8"/>
     </row>
     <row r="860" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C860" s="18"/>
+      <c r="C860" s="8"/>
     </row>
     <row r="861" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C861" s="18"/>
+      <c r="C861" s="8"/>
     </row>
     <row r="862" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C862" s="18"/>
+      <c r="C862" s="8"/>
     </row>
     <row r="863" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C863" s="18"/>
+      <c r="C863" s="8"/>
     </row>
     <row r="864" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C864" s="18"/>
+      <c r="C864" s="8"/>
     </row>
     <row r="865" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C865" s="18"/>
+      <c r="C865" s="8"/>
     </row>
     <row r="866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C866" s="18"/>
+      <c r="C866" s="8"/>
     </row>
     <row r="867" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C867" s="18"/>
+      <c r="C867" s="8"/>
     </row>
     <row r="868" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C868" s="18"/>
+      <c r="C868" s="8"/>
     </row>
     <row r="869" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C869" s="18"/>
+      <c r="C869" s="8"/>
     </row>
     <row r="870" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C870" s="18"/>
+      <c r="C870" s="8"/>
     </row>
     <row r="871" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C871" s="18"/>
+      <c r="C871" s="8"/>
     </row>
     <row r="872" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C872" s="18"/>
+      <c r="C872" s="8"/>
     </row>
     <row r="873" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C873" s="18"/>
+      <c r="C873" s="8"/>
     </row>
     <row r="874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C874" s="18"/>
+      <c r="C874" s="8"/>
     </row>
     <row r="875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C875" s="18"/>
+      <c r="C875" s="8"/>
     </row>
     <row r="876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C876" s="18"/>
+      <c r="C876" s="8"/>
     </row>
     <row r="877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C877" s="18"/>
+      <c r="C877" s="8"/>
     </row>
     <row r="878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C878" s="18"/>
+      <c r="C878" s="8"/>
     </row>
     <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C879" s="18"/>
+      <c r="C879" s="8"/>
     </row>
     <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C880" s="18"/>
+      <c r="C880" s="8"/>
     </row>
     <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C881" s="18"/>
+      <c r="C881" s="8"/>
     </row>
     <row r="882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C882" s="18"/>
+      <c r="C882" s="8"/>
     </row>
     <row r="883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C883" s="18"/>
+      <c r="C883" s="8"/>
     </row>
     <row r="884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C884" s="18"/>
+      <c r="C884" s="8"/>
     </row>
     <row r="885" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C885" s="18"/>
+      <c r="C885" s="8"/>
     </row>
     <row r="886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C886" s="18"/>
+      <c r="C886" s="8"/>
     </row>
     <row r="887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C887" s="18"/>
+      <c r="C887" s="8"/>
     </row>
     <row r="888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C888" s="18"/>
+      <c r="C888" s="8"/>
     </row>
     <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C889" s="18"/>
+      <c r="C889" s="8"/>
     </row>
     <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C890" s="18"/>
+      <c r="C890" s="8"/>
     </row>
     <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C891" s="18"/>
+      <c r="C891" s="8"/>
     </row>
     <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C892" s="18"/>
+      <c r="C892" s="8"/>
     </row>
     <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C893" s="18"/>
+      <c r="C893" s="8"/>
     </row>
     <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C894" s="18"/>
+      <c r="C894" s="8"/>
     </row>
     <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C895" s="18"/>
+      <c r="C895" s="8"/>
     </row>
     <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C896" s="18"/>
+      <c r="C896" s="8"/>
     </row>
     <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C897" s="18"/>
+      <c r="C897" s="8"/>
     </row>
     <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C898" s="18"/>
+      <c r="C898" s="8"/>
     </row>
     <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C899" s="18"/>
+      <c r="C899" s="8"/>
     </row>
     <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C900" s="18"/>
+      <c r="C900" s="8"/>
     </row>
     <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C901" s="18"/>
+      <c r="C901" s="8"/>
     </row>
     <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C902" s="18"/>
+      <c r="C902" s="8"/>
     </row>
     <row r="903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C903" s="18"/>
+      <c r="C903" s="8"/>
     </row>
     <row r="904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C904" s="18"/>
+      <c r="C904" s="8"/>
     </row>
     <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C905" s="18"/>
+      <c r="C905" s="8"/>
     </row>
     <row r="906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C906" s="18"/>
+      <c r="C906" s="8"/>
     </row>
     <row r="907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C907" s="18"/>
+      <c r="C907" s="8"/>
     </row>
     <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C908" s="18"/>
+      <c r="C908" s="8"/>
     </row>
     <row r="909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C909" s="18"/>
+      <c r="C909" s="8"/>
     </row>
     <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C910" s="18"/>
+      <c r="C910" s="8"/>
     </row>
     <row r="911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C911" s="18"/>
+      <c r="C911" s="8"/>
     </row>
     <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C912" s="18"/>
+      <c r="C912" s="8"/>
     </row>
     <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C913" s="18"/>
+      <c r="C913" s="8"/>
     </row>
     <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C914" s="18"/>
+      <c r="C914" s="8"/>
     </row>
     <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C915" s="18"/>
+      <c r="C915" s="8"/>
     </row>
     <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C916" s="18"/>
+      <c r="C916" s="8"/>
     </row>
     <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C917" s="18"/>
+      <c r="C917" s="8"/>
     </row>
     <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C918" s="18"/>
+      <c r="C918" s="8"/>
     </row>
     <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C919" s="18"/>
+      <c r="C919" s="8"/>
     </row>
     <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C920" s="18"/>
+      <c r="C920" s="8"/>
     </row>
     <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C921" s="18"/>
+      <c r="C921" s="8"/>
     </row>
     <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C922" s="18"/>
+      <c r="C922" s="8"/>
     </row>
     <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C923" s="18"/>
+      <c r="C923" s="8"/>
     </row>
     <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C924" s="18"/>
+      <c r="C924" s="8"/>
     </row>
     <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C925" s="18"/>
+      <c r="C925" s="8"/>
     </row>
     <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C926" s="18"/>
+      <c r="C926" s="8"/>
     </row>
     <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C927" s="18"/>
+      <c r="C927" s="8"/>
     </row>
     <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C928" s="18"/>
+      <c r="C928" s="8"/>
     </row>
     <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C929" s="18"/>
+      <c r="C929" s="8"/>
     </row>
     <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C930" s="18"/>
+      <c r="C930" s="8"/>
     </row>
     <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C931" s="18"/>
+      <c r="C931" s="8"/>
     </row>
     <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C932" s="18"/>
+      <c r="C932" s="8"/>
     </row>
     <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C933" s="18"/>
+      <c r="C933" s="8"/>
     </row>
     <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C934" s="18"/>
+      <c r="C934" s="8"/>
     </row>
     <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C935" s="18"/>
+      <c r="C935" s="8"/>
     </row>
     <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C936" s="18"/>
+      <c r="C936" s="8"/>
     </row>
     <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C937" s="18"/>
+      <c r="C937" s="8"/>
     </row>
     <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C938" s="18"/>
+      <c r="C938" s="8"/>
     </row>
     <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C939" s="18"/>
+      <c r="C939" s="8"/>
     </row>
     <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C940" s="18"/>
+      <c r="C940" s="8"/>
     </row>
     <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C941" s="18"/>
+      <c r="C941" s="8"/>
     </row>
     <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C942" s="18"/>
+      <c r="C942" s="8"/>
     </row>
     <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C943" s="18"/>
+      <c r="C943" s="8"/>
     </row>
     <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C944" s="18"/>
+      <c r="C944" s="8"/>
     </row>
     <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C945" s="18"/>
+      <c r="C945" s="8"/>
     </row>
     <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C946" s="18"/>
+      <c r="C946" s="8"/>
     </row>
     <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C947" s="18"/>
+      <c r="C947" s="8"/>
     </row>
     <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C948" s="18"/>
+      <c r="C948" s="8"/>
     </row>
     <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C949" s="18"/>
+      <c r="C949" s="8"/>
     </row>
     <row r="950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C950" s="18"/>
+      <c r="C950" s="8"/>
     </row>
     <row r="951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C951" s="18"/>
+      <c r="C951" s="8"/>
     </row>
     <row r="952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C952" s="18"/>
+      <c r="C952" s="8"/>
     </row>
     <row r="953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C953" s="18"/>
+      <c r="C953" s="8"/>
     </row>
     <row r="954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C954" s="18"/>
+      <c r="C954" s="8"/>
     </row>
     <row r="955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C955" s="18"/>
+      <c r="C955" s="8"/>
     </row>
     <row r="956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C956" s="18"/>
+      <c r="C956" s="8"/>
     </row>
     <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C957" s="18"/>
+      <c r="C957" s="8"/>
     </row>
     <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C958" s="18"/>
+      <c r="C958" s="8"/>
     </row>
     <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C959" s="18"/>
+      <c r="C959" s="8"/>
     </row>
     <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C960" s="18"/>
+      <c r="C960" s="8"/>
     </row>
     <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C961" s="18"/>
+      <c r="C961" s="8"/>
     </row>
     <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C962" s="18"/>
+      <c r="C962" s="8"/>
     </row>
     <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C963" s="18"/>
+      <c r="C963" s="8"/>
     </row>
     <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C964" s="18"/>
+      <c r="C964" s="8"/>
     </row>
     <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C965" s="18"/>
+      <c r="C965" s="8"/>
     </row>
     <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C966" s="18"/>
+      <c r="C966" s="8"/>
     </row>
     <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C967" s="18"/>
+      <c r="C967" s="8"/>
     </row>
     <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C968" s="18"/>
+      <c r="C968" s="8"/>
     </row>
     <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C969" s="18"/>
+      <c r="C969" s="8"/>
     </row>
     <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C970" s="18"/>
+      <c r="C970" s="8"/>
     </row>
     <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C971" s="18"/>
+      <c r="C971" s="8"/>
     </row>
     <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C972" s="18"/>
+      <c r="C972" s="8"/>
     </row>
     <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C973" s="18"/>
+      <c r="C973" s="8"/>
     </row>
     <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C974" s="18"/>
+      <c r="C974" s="8"/>
     </row>
     <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C975" s="18"/>
+      <c r="C975" s="8"/>
     </row>
     <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C976" s="18"/>
+      <c r="C976" s="8"/>
     </row>
     <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C977" s="18"/>
+      <c r="C977" s="8"/>
     </row>
     <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C978" s="18"/>
+      <c r="C978" s="8"/>
     </row>
     <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C979" s="18"/>
+      <c r="C979" s="8"/>
     </row>
     <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C980" s="18"/>
+      <c r="C980" s="8"/>
     </row>
     <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C981" s="18"/>
+      <c r="C981" s="8"/>
     </row>
     <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C982" s="18"/>
+      <c r="C982" s="8"/>
     </row>
     <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C983" s="18"/>
+      <c r="C983" s="8"/>
     </row>
     <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C984" s="18"/>
+      <c r="C984" s="8"/>
     </row>
     <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C985" s="18"/>
+      <c r="C985" s="8"/>
     </row>
     <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C986" s="18"/>
+      <c r="C986" s="8"/>
     </row>
     <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C987" s="18"/>
+      <c r="C987" s="8"/>
     </row>
     <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C988" s="18"/>
+      <c r="C988" s="8"/>
     </row>
     <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C989" s="18"/>
+      <c r="C989" s="8"/>
     </row>
     <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C990" s="18"/>
+      <c r="C990" s="8"/>
     </row>
     <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C991" s="18"/>
+      <c r="C991" s="8"/>
     </row>
     <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C992" s="18"/>
+      <c r="C992" s="8"/>
     </row>
     <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C993" s="18"/>
+      <c r="C993" s="8"/>
     </row>
     <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C994" s="18"/>
+      <c r="C994" s="8"/>
     </row>
     <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C995" s="18"/>
+      <c r="C995" s="8"/>
     </row>
     <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C996" s="18"/>
+      <c r="C996" s="8"/>
     </row>
     <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C997" s="18"/>
+      <c r="C997" s="8"/>
     </row>
     <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C998" s="18"/>
+      <c r="C998" s="8"/>
     </row>
     <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C999" s="18"/>
+      <c r="C999" s="8"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E14">
+    <cfRule type="cellIs" priority="2" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>Sheet_rec!$D2</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>Sheet_rec!$D$2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>